<commit_message>
Added rttr submodule, folder restructuring
</commit_message>
<xml_diff>
--- a/measurements/inital_rtt_test/rtt_test_0.xlsx
+++ b/measurements/inital_rtt_test/rtt_test_0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik Nyholm\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik Nyholm\Documents\NTNU\Master\Project\system_on_sheep\measurements\inital_rtt_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79F7AB5-D607-4196-8068-CDDB6F649B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF77CE2-6CC4-4092-BA5E-034B2AFEC805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="16875" windowHeight="10522" xr2:uid="{121F26D3-F8F5-4117-B270-8C0302727CE4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{121F26D3-F8F5-4117-B270-8C0302727CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="128" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>flylinje dist [m]</t>
   </si>
@@ -67,6 +67,33 @@
   </si>
   <si>
     <t>error [m]</t>
+  </si>
+  <si>
+    <t>printed rtt dist [m]</t>
+  </si>
+  <si>
+    <t>ticks * (light speed) / (2 * timer frequency)</t>
+  </si>
+  <si>
+    <t>speed of light</t>
+  </si>
+  <si>
+    <t>timer freq</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>error printed[m]</t>
+  </si>
+  <si>
+    <t>avg ticks</t>
+  </si>
+  <si>
+    <t>avg ticks dist [m]</t>
+  </si>
+  <si>
+    <t>error avg ticks dist [m]</t>
   </si>
 </sst>
 </file>
@@ -184,7 +211,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>error [m]</c:v>
+                  <c:v>error printed[m]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -437,6 +464,318 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'128'!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>error avg ticks dist [m]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'128'!$G$5:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-084B-4306-93D6-A487DDB5E7BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="648027640"/>
+        <c:axId val="648025400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="648027640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="648025400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="648025400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="648027640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -860,6 +1199,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1866,20 +2245,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>150019</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>509588</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>169069</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>178594</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>16669</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1899,6 +2781,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>459580</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>497680</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>26194</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83C552AD-64C8-47FC-BE31-C6068A588C0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2245,22 +3163,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10893923-ADF5-4D29-AD8F-1FEC9F2AB6BC}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.86328125" customWidth="1"/>
     <col min="2" max="2" width="13.19921875" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" customWidth="1"/>
-    <col min="5" max="5" width="7.19921875" customWidth="1"/>
-    <col min="6" max="6" width="11.46484375" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" customWidth="1"/>
+    <col min="4" max="4" width="15.06640625" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2269,7 +3189,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2277,19 +3197,28 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2304,13 +3233,24 @@
         <v>-1</v>
       </c>
       <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <f>ROUND(E5*$B$28,0)</f>
+        <v>103</v>
+      </c>
+      <c r="G5">
+        <f>F5-B5</f>
+        <v>3</v>
+      </c>
+      <c r="H5">
         <v>128</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>50</v>
       </c>
@@ -2322,17 +3262,28 @@
         <v>108</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D23" si="0">C6-B6</f>
+        <f>C6-B6</f>
         <v>-4</v>
       </c>
       <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <f>ROUND(E6*$B$28,0)</f>
+        <v>112</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G23" si="0">F6-B6</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>128</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>100</v>
       </c>
@@ -2344,17 +3295,28 @@
         <v>144</v>
       </c>
       <c r="D7">
+        <f>C7-B7</f>
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <f>ROUND(E7*$B$28,0)</f>
+        <v>150</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="H7">
         <v>128</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>150</v>
       </c>
@@ -2366,17 +3328,28 @@
         <v>180</v>
       </c>
       <c r="D8">
+        <f>C8-B8</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <f>ROUND(E8*$B$28,0)</f>
+        <v>187</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="H8">
         <v>128</v>
       </c>
-      <c r="F8">
+      <c r="I8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>200</v>
       </c>
@@ -2388,17 +3361,28 @@
         <v>225</v>
       </c>
       <c r="D9">
+        <f>C9-B9</f>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <f>ROUND(E9*$B$28,0)</f>
+        <v>234</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="H9">
         <v>128</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>250</v>
       </c>
@@ -2410,17 +3394,28 @@
         <v>279</v>
       </c>
       <c r="D10">
+        <f>C10-B10</f>
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>31</v>
+      </c>
+      <c r="F10">
+        <f>ROUND(E10*$B$28,0)</f>
+        <v>290</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E10">
+        <v>21</v>
+      </c>
+      <c r="H10">
         <v>127</v>
       </c>
-      <c r="F10">
+      <c r="I10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>300</v>
       </c>
@@ -2432,17 +3427,28 @@
         <v>297</v>
       </c>
       <c r="D11">
+        <f>C11-B11</f>
+        <v>-19</v>
+      </c>
+      <c r="E11">
+        <v>33</v>
+      </c>
+      <c r="F11">
+        <f>ROUND(E11*$B$28,0)</f>
+        <v>309</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>-19</v>
-      </c>
-      <c r="E11">
+        <v>-7</v>
+      </c>
+      <c r="H11">
         <v>128</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>350</v>
       </c>
@@ -2454,17 +3460,28 @@
         <v>360</v>
       </c>
       <c r="D12">
+        <f>C12-B12</f>
+        <v>-4</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <f>ROUND(E12*$B$28,0)</f>
+        <v>375</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="H12">
         <v>128</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>400</v>
       </c>
@@ -2476,17 +3493,28 @@
         <v>405</v>
       </c>
       <c r="D13">
+        <f>C13-B13</f>
+        <v>-7</v>
+      </c>
+      <c r="E13">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <f>ROUND(E13*$B$28,0)</f>
+        <v>422</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>-7</v>
-      </c>
-      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="H13">
         <v>128</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>450</v>
       </c>
@@ -2498,17 +3526,28 @@
         <v>450</v>
       </c>
       <c r="D14">
+        <f>C14-B14</f>
+        <v>-11</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <f>ROUND(E14*$B$28,0)</f>
+        <v>468</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
-        <v>-11</v>
-      </c>
-      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="H14">
         <v>128</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>500</v>
       </c>
@@ -2520,17 +3559,28 @@
         <v>504</v>
       </c>
       <c r="D15">
+        <f>C15-B15</f>
+        <v>-6</v>
+      </c>
+      <c r="E15">
+        <v>56</v>
+      </c>
+      <c r="F15">
+        <f>ROUND(E15*$B$28,0)</f>
+        <v>525</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
-      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="H15">
         <v>127</v>
       </c>
-      <c r="F15">
+      <c r="I15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>550</v>
       </c>
@@ -2542,17 +3592,28 @@
         <v>540</v>
       </c>
       <c r="D16">
+        <f>C16-B16</f>
+        <v>-19</v>
+      </c>
+      <c r="E16">
+        <v>60</v>
+      </c>
+      <c r="F16">
+        <f>ROUND(E16*$B$28,0)</f>
+        <v>562</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="0"/>
-        <v>-19</v>
-      </c>
-      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="H16">
         <v>125</v>
       </c>
-      <c r="F16">
+      <c r="I16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>600</v>
       </c>
@@ -2564,17 +3625,28 @@
         <v>594</v>
       </c>
       <c r="D17">
+        <f>C17-B17</f>
+        <v>-14</v>
+      </c>
+      <c r="E17">
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <f>ROUND(E17*$B$28,0)</f>
+        <v>618</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="0"/>
-        <v>-14</v>
-      </c>
-      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="H17">
         <v>128</v>
       </c>
-      <c r="F17">
+      <c r="I17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>650</v>
       </c>
@@ -2586,17 +3658,28 @@
         <v>639</v>
       </c>
       <c r="D18">
+        <f>C18-B18</f>
+        <v>-19</v>
+      </c>
+      <c r="E18">
+        <v>71</v>
+      </c>
+      <c r="F18">
+        <f>ROUND(E18*$B$28,0)</f>
+        <v>665</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="0"/>
-        <v>-19</v>
-      </c>
-      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="H18">
         <v>128</v>
       </c>
-      <c r="F18">
+      <c r="I18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>700</v>
       </c>
@@ -2608,17 +3691,28 @@
         <v>693</v>
       </c>
       <c r="D19">
+        <f>C19-B19</f>
+        <v>-14</v>
+      </c>
+      <c r="E19">
+        <v>77</v>
+      </c>
+      <c r="F19">
+        <f>ROUND(E19*$B$28,0)</f>
+        <v>721</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="0"/>
-        <v>-14</v>
-      </c>
-      <c r="E19">
+        <v>14</v>
+      </c>
+      <c r="H19">
         <v>127</v>
       </c>
-      <c r="F19">
+      <c r="I19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>750</v>
       </c>
@@ -2630,17 +3724,28 @@
         <v>738</v>
       </c>
       <c r="D20">
+        <f>C20-B20</f>
+        <v>-19</v>
+      </c>
+      <c r="E20">
+        <v>82</v>
+      </c>
+      <c r="F20">
+        <f>ROUND(E20*$B$28,0)</f>
+        <v>768</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="0"/>
-        <v>-19</v>
-      </c>
-      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="H20">
         <v>19</v>
       </c>
-      <c r="F20">
+      <c r="I20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>800</v>
       </c>
@@ -2652,17 +3757,28 @@
         <v>792</v>
       </c>
       <c r="D21">
+        <f>C21-B21</f>
+        <v>-14</v>
+      </c>
+      <c r="E21">
+        <v>88</v>
+      </c>
+      <c r="F21">
+        <f>ROUND(E21*$B$28,0)</f>
+        <v>824</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="0"/>
-        <v>-14</v>
-      </c>
-      <c r="E21">
+        <v>18</v>
+      </c>
+      <c r="H21">
         <v>127</v>
       </c>
-      <c r="F21">
+      <c r="I21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>850</v>
       </c>
@@ -2674,17 +3790,28 @@
         <v>846</v>
       </c>
       <c r="D22">
+        <f>C22-B22</f>
+        <v>-10</v>
+      </c>
+      <c r="E22">
+        <v>94</v>
+      </c>
+      <c r="F22">
+        <f>ROUND(E22*$B$28,0)</f>
+        <v>881</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-      <c r="E22">
+        <v>25</v>
+      </c>
+      <c r="H22">
         <v>123</v>
       </c>
-      <c r="F22">
+      <c r="I22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>900</v>
       </c>
@@ -2696,50 +3823,55 @@
         <v>882</v>
       </c>
       <c r="D23">
+        <f>C23-B23</f>
+        <v>-24</v>
+      </c>
+      <c r="E23">
+        <v>98</v>
+      </c>
+      <c r="F23">
+        <f>ROUND(E23*$B$28,0)</f>
+        <v>918</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="0"/>
-        <v>-24</v>
-      </c>
-      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="H23">
         <v>115</v>
       </c>
-      <c r="F23">
+      <c r="I23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>950</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="1"/>
-        <v>955</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>1000</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="1"/>
-        <v>1005</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" t="s">
-        <v>5</v>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>299792458</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>16000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <f>B26/(2*B27)</f>
+        <v>9.3685143125000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>